<commit_message>
updated benchmarks and output
</commit_message>
<xml_diff>
--- a/PrimesGaps-C/benchmarks/Benchmark.xlsx
+++ b/PrimesGaps-C/benchmarks/Benchmark.xlsx
@@ -1467,7 +1467,7 @@
   <dimension ref="A18:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1653,11 +1653,11 @@
         <v>32</v>
       </c>
       <c r="C27" s="2">
-        <v>22961.895399000001</v>
+        <v>33723.286738000003</v>
       </c>
       <c r="D27" s="3">
         <f t="shared" si="0"/>
-        <v>382.69825665000002</v>
+        <v>562.05477896666673</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="5" t="s">
@@ -1670,11 +1670,11 @@
         <v>64</v>
       </c>
       <c r="C28" s="1">
-        <v>11632.860207</v>
+        <v>17065.508472000001</v>
       </c>
       <c r="D28" s="3">
         <f t="shared" si="0"/>
-        <v>193.88100345000001</v>
+        <v>284.42514120000004</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="5"/>

</xml_diff>